<commit_message>
optimize reflect set slice functions add ci test update markdown badges
</commit_message>
<xml_diff>
--- a/example/xlsx/people.xlsx
+++ b/example/xlsx/people.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -31,15 +31,6 @@
   </si>
   <si>
     <t>address</t>
-  </si>
-  <si>
-    <t>n-0</t>
-  </si>
-  <si>
-    <t>school-0</t>
-  </si>
-  <si>
-    <t>hali-0</t>
   </si>
   <si>
     <t>n-1</t>
@@ -442,7 +433,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -482,7 +473,7 @@
         <v>1.2345678900</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -499,7 +490,7 @@
         <v>1.2345678900</v>
       </c>
       <c r="C3" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -516,7 +507,7 @@
         <v>1.2345678900</v>
       </c>
       <c r="C4" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -533,30 +524,13 @@
         <v>1.2345678900</v>
       </c>
       <c r="C5" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.2345678900</v>
-      </c>
-      <c r="C6" s="1">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add ci test; fix csv dump bug
</commit_message>
<xml_diff>
--- a/example/xlsx/people.xlsx
+++ b/example/xlsx/people.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -31,15 +31,6 @@
   </si>
   <si>
     <t>address</t>
-  </si>
-  <si>
-    <t>n-0</t>
-  </si>
-  <si>
-    <t>school-0</t>
-  </si>
-  <si>
-    <t>hali-0</t>
   </si>
   <si>
     <t>n-1</t>
@@ -442,7 +433,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -482,7 +473,7 @@
         <v>1.2345678900</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -499,7 +490,7 @@
         <v>1.2345678900</v>
       </c>
       <c r="C3" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -516,7 +507,7 @@
         <v>1.2345678900</v>
       </c>
       <c r="C4" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -533,30 +524,13 @@
         <v>1.2345678900</v>
       </c>
       <c r="C5" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.2345678900</v>
-      </c>
-      <c r="C6" s="1">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>